<commit_message>
add some experimental routines
</commit_message>
<xml_diff>
--- a/doc/ssememo.xlsx
+++ b/doc/ssememo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="11355" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="11355" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="15" sheetId="16" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2222" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="37">
   <si>
     <t>a</t>
     <phoneticPr fontId="1"/>
@@ -159,6 +159,30 @@
     <t>a</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -189,9 +213,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -203,11 +236,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2478,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AT15" activeCellId="1" sqref="AB56:AX77 AT15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="13.5"/>
@@ -12276,10 +12312,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:AI44"/>
+  <dimension ref="A2:DH58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AO37" sqref="AO37"/>
+    <sheetView topLeftCell="BE29" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="BU36" sqref="BU36:DH43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5" defaultRowHeight="13.5"/>
@@ -12287,7 +12323,7 @@
     <col min="1" max="16384" width="2.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:84">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -12388,7 +12424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:84">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -12489,7 +12525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:84">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -12590,7 +12626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:84">
       <c r="C6" s="1">
         <v>0</v>
       </c>
@@ -12687,8 +12723,32 @@
       <c r="AI6" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:35">
+      <c r="BC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD6" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE6" s="1">
+        <v>2</v>
+      </c>
+      <c r="BF6" s="1">
+        <v>3</v>
+      </c>
+      <c r="BG6" s="1">
+        <v>4</v>
+      </c>
+      <c r="BH6" s="1">
+        <v>5</v>
+      </c>
+      <c r="BI6" s="1">
+        <v>6</v>
+      </c>
+      <c r="BJ6" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:84">
       <c r="D7" s="1">
         <v>1</v>
       </c>
@@ -12773,8 +12833,29 @@
       <c r="AI7" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:35">
+      <c r="BD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF7" s="1">
+        <v>2</v>
+      </c>
+      <c r="BG7" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH7" s="1">
+        <v>4</v>
+      </c>
+      <c r="BI7" s="1">
+        <v>5</v>
+      </c>
+      <c r="BJ7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:84">
       <c r="E8" s="1">
         <v>2</v>
       </c>
@@ -12847,8 +12928,26 @@
       <c r="AI8" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:35">
+      <c r="BE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG8" s="1">
+        <v>2</v>
+      </c>
+      <c r="BH8" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI8" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:84">
       <c r="F9" s="1">
         <v>3</v>
       </c>
@@ -12909,8 +13008,23 @@
       <c r="AI9" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:35">
+      <c r="BF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH9" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI9" s="1">
+        <v>3</v>
+      </c>
+      <c r="BJ9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:84">
       <c r="G10" s="1">
         <v>4</v>
       </c>
@@ -12959,8 +13073,44 @@
       <c r="AI10" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:35">
+      <c r="BG10" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH10" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI10" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ10" s="1">
+        <v>3</v>
+      </c>
+      <c r="BY10" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ10" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CB10" s="1">
+        <v>3</v>
+      </c>
+      <c r="CC10" s="1">
+        <v>4</v>
+      </c>
+      <c r="CD10" s="1">
+        <v>5</v>
+      </c>
+      <c r="CE10" s="1">
+        <v>6</v>
+      </c>
+      <c r="CF10" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:84">
       <c r="H11" s="1">
         <v>5</v>
       </c>
@@ -12997,8 +13147,38 @@
       <c r="AI11" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:35">
+      <c r="BH11" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ11" s="1">
+        <v>2</v>
+      </c>
+      <c r="BZ11" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA11" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB11" s="1">
+        <v>2</v>
+      </c>
+      <c r="CC11" s="1">
+        <v>3</v>
+      </c>
+      <c r="CD11" s="1">
+        <v>4</v>
+      </c>
+      <c r="CE11" s="1">
+        <v>5</v>
+      </c>
+      <c r="CF11" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:84">
       <c r="I12" s="1">
         <v>6</v>
       </c>
@@ -13023,8 +13203,32 @@
       <c r="AI12" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:35">
+      <c r="BI12" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA12" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB12" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC12" s="1">
+        <v>2</v>
+      </c>
+      <c r="CD12" s="1">
+        <v>3</v>
+      </c>
+      <c r="CE12" s="1">
+        <v>4</v>
+      </c>
+      <c r="CF12" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:84">
       <c r="J13" s="1">
         <v>7</v>
       </c>
@@ -13037,8 +13241,64 @@
       <c r="AI13" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:35">
+      <c r="BJ13" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB13" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC13" s="1">
+        <v>1</v>
+      </c>
+      <c r="CD13" s="1">
+        <v>2</v>
+      </c>
+      <c r="CE13" s="1">
+        <v>3</v>
+      </c>
+      <c r="CF13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:84">
+      <c r="BK14" s="1">
+        <v>8</v>
+      </c>
+      <c r="BL14" s="1">
+        <v>9</v>
+      </c>
+      <c r="BM14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BN14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BO14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BP14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BQ14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="BR14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="CC14" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD14" s="1">
+        <v>1</v>
+      </c>
+      <c r="CE14" s="1">
+        <v>2</v>
+      </c>
+      <c r="CF14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:84">
       <c r="C15" s="1">
         <v>3</v>
       </c>
@@ -13135,8 +13395,38 @@
       <c r="AI15" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:35">
+      <c r="BL15" s="1">
+        <v>8</v>
+      </c>
+      <c r="BM15" s="1">
+        <v>9</v>
+      </c>
+      <c r="BN15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BO15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BP15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BQ15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BR15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="CD15" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE15" s="1">
+        <v>1</v>
+      </c>
+      <c r="CF15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:84">
       <c r="D16" s="1">
         <v>2</v>
       </c>
@@ -13221,8 +13511,32 @@
       <c r="AI16" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:35">
+      <c r="BM16" s="1">
+        <v>8</v>
+      </c>
+      <c r="BN16" s="1">
+        <v>9</v>
+      </c>
+      <c r="BO16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BP16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BQ16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="CE16" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:89">
       <c r="E17" s="1">
         <v>1</v>
       </c>
@@ -13295,8 +13609,26 @@
       <c r="AI17" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:35">
+      <c r="BN17" s="1">
+        <v>8</v>
+      </c>
+      <c r="BO17" s="1">
+        <v>9</v>
+      </c>
+      <c r="BP17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BQ17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BR17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:89">
       <c r="F18" s="1">
         <v>0</v>
       </c>
@@ -13357,8 +13689,20 @@
       <c r="AI18" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:35">
+      <c r="BO18" s="1">
+        <v>8</v>
+      </c>
+      <c r="BP18" s="1">
+        <v>9</v>
+      </c>
+      <c r="BQ18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BR18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:89">
       <c r="G19" s="1">
         <v>1</v>
       </c>
@@ -13407,8 +13751,53 @@
       <c r="AI19" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:35">
+      <c r="AU19" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV19" s="1">
+        <v>4</v>
+      </c>
+      <c r="BP19" s="1">
+        <v>8</v>
+      </c>
+      <c r="BQ19" s="1">
+        <v>9</v>
+      </c>
+      <c r="BR19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BY19" s="1">
+        <v>4</v>
+      </c>
+      <c r="BZ19" s="1">
+        <v>5</v>
+      </c>
+      <c r="CA19" s="1">
+        <v>6</v>
+      </c>
+      <c r="CB19" s="1">
+        <v>7</v>
+      </c>
+      <c r="CC19" s="1">
+        <v>8</v>
+      </c>
+      <c r="CE19" s="1">
+        <v>5</v>
+      </c>
+      <c r="CF19" s="1">
+        <v>6</v>
+      </c>
+      <c r="CG19" s="1">
+        <v>7</v>
+      </c>
+      <c r="CH19" s="1">
+        <v>8</v>
+      </c>
+      <c r="CI19" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:89">
       <c r="H20" s="1">
         <v>2</v>
       </c>
@@ -13445,8 +13834,50 @@
       <c r="AI20" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:35">
+      <c r="AU20" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV20" s="1">
+        <v>3</v>
+      </c>
+      <c r="BQ20" s="1">
+        <v>8</v>
+      </c>
+      <c r="BR20" s="1">
+        <v>9</v>
+      </c>
+      <c r="BY20" s="1">
+        <v>3</v>
+      </c>
+      <c r="BZ20" s="1">
+        <v>4</v>
+      </c>
+      <c r="CA20" s="1">
+        <v>5</v>
+      </c>
+      <c r="CB20" s="1">
+        <v>6</v>
+      </c>
+      <c r="CC20" s="1">
+        <v>7</v>
+      </c>
+      <c r="CE20" s="1">
+        <v>4</v>
+      </c>
+      <c r="CF20" s="1">
+        <v>5</v>
+      </c>
+      <c r="CG20" s="1">
+        <v>6</v>
+      </c>
+      <c r="CH20" s="1">
+        <v>7</v>
+      </c>
+      <c r="CI20" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:89">
       <c r="I21" s="1">
         <v>3</v>
       </c>
@@ -13471,8 +13902,47 @@
       <c r="AI21" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:35">
+      <c r="AU21" s="1">
+        <v>2</v>
+      </c>
+      <c r="AV21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BR21" s="1">
+        <v>8</v>
+      </c>
+      <c r="BY21" s="1">
+        <v>2</v>
+      </c>
+      <c r="BZ21" s="1">
+        <v>3</v>
+      </c>
+      <c r="CA21" s="1">
+        <v>4</v>
+      </c>
+      <c r="CB21" s="1">
+        <v>5</v>
+      </c>
+      <c r="CC21" s="1">
+        <v>6</v>
+      </c>
+      <c r="CE21" s="1">
+        <v>3</v>
+      </c>
+      <c r="CF21" s="1">
+        <v>4</v>
+      </c>
+      <c r="CG21" s="1">
+        <v>5</v>
+      </c>
+      <c r="CH21" s="1">
+        <v>6</v>
+      </c>
+      <c r="CI21" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:89">
       <c r="J22" s="1">
         <v>4</v>
       </c>
@@ -13485,8 +13955,124 @@
       <c r="AI22" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:35">
+      <c r="AU22" s="1">
+        <v>1</v>
+      </c>
+      <c r="BY22" s="1">
+        <v>1</v>
+      </c>
+      <c r="BZ22" s="1">
+        <v>2</v>
+      </c>
+      <c r="CA22" s="1">
+        <v>3</v>
+      </c>
+      <c r="CB22" s="1">
+        <v>4</v>
+      </c>
+      <c r="CC22" s="1">
+        <v>5</v>
+      </c>
+      <c r="CE22" s="1">
+        <v>2</v>
+      </c>
+      <c r="CF22" s="1">
+        <v>3</v>
+      </c>
+      <c r="CG22" s="1">
+        <v>4</v>
+      </c>
+      <c r="CH22" s="1">
+        <v>5</v>
+      </c>
+      <c r="CI22" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:89">
+      <c r="AU23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD23" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE23" s="1">
+        <v>2</v>
+      </c>
+      <c r="BF23" s="1">
+        <v>3</v>
+      </c>
+      <c r="BG23" s="1">
+        <v>4</v>
+      </c>
+      <c r="BH23" s="1">
+        <v>5</v>
+      </c>
+      <c r="BI23" s="1">
+        <v>6</v>
+      </c>
+      <c r="BJ23" s="1">
+        <v>7</v>
+      </c>
+      <c r="BK23" s="1">
+        <v>8</v>
+      </c>
+      <c r="BL23" s="1">
+        <v>9</v>
+      </c>
+      <c r="BM23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BN23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BO23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BP23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BQ23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="BR23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BY23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ23" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA23" s="1">
+        <v>2</v>
+      </c>
+      <c r="CB23" s="1">
+        <v>3</v>
+      </c>
+      <c r="CC23" s="1">
+        <v>4</v>
+      </c>
+      <c r="CE23" s="1">
+        <v>1</v>
+      </c>
+      <c r="CF23" s="1">
+        <v>2</v>
+      </c>
+      <c r="CG23" s="1">
+        <v>3</v>
+      </c>
+      <c r="CH23" s="1">
+        <v>4</v>
+      </c>
+      <c r="CI23" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:89">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -13586,8 +14172,50 @@
       <c r="AI24" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:35">
+      <c r="BD24" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE24" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF24" s="1">
+        <v>2</v>
+      </c>
+      <c r="BG24" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH24" s="1">
+        <v>4</v>
+      </c>
+      <c r="BI24" s="1">
+        <v>5</v>
+      </c>
+      <c r="BJ24" s="1">
+        <v>6</v>
+      </c>
+      <c r="BL24" s="1">
+        <v>8</v>
+      </c>
+      <c r="BM24" s="1">
+        <v>9</v>
+      </c>
+      <c r="BN24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BP24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BQ24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BR24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:89">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -13687,8 +14315,86 @@
       <c r="AI25" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:35">
+      <c r="AU25" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV25" s="1">
+        <v>3</v>
+      </c>
+      <c r="BD25" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE25" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF25" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG25" s="1">
+        <v>2</v>
+      </c>
+      <c r="BH25" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI25" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ25" s="1">
+        <v>5</v>
+      </c>
+      <c r="BL25" s="1">
+        <v>8</v>
+      </c>
+      <c r="BM25" s="1">
+        <v>8</v>
+      </c>
+      <c r="BN25" s="1">
+        <v>9</v>
+      </c>
+      <c r="BO25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BQ25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BU25" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV25" s="1">
+        <v>1</v>
+      </c>
+      <c r="BW25" s="1">
+        <v>2</v>
+      </c>
+      <c r="BX25" s="1">
+        <v>3</v>
+      </c>
+      <c r="BY25" s="1">
+        <v>4</v>
+      </c>
+      <c r="BZ25" s="1">
+        <v>5</v>
+      </c>
+      <c r="CA25" s="1">
+        <v>6</v>
+      </c>
+      <c r="CB25" s="1">
+        <v>7</v>
+      </c>
+      <c r="CC25" s="1">
+        <v>8</v>
+      </c>
+      <c r="CD25" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:89">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -13788,8 +14494,145 @@
       <c r="AI26" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:35">
+      <c r="AU26" s="1">
+        <v>2</v>
+      </c>
+      <c r="AV26" s="1">
+        <v>2</v>
+      </c>
+      <c r="BE26" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF26" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG26" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH26" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI26" s="1">
+        <v>3</v>
+      </c>
+      <c r="BJ26" s="1">
+        <v>4</v>
+      </c>
+      <c r="BM26" s="1">
+        <v>9</v>
+      </c>
+      <c r="BN26" s="1">
+        <v>8</v>
+      </c>
+      <c r="BO26" s="1">
+        <v>9</v>
+      </c>
+      <c r="BP26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BQ26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BR26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BV26" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW26" s="1">
+        <v>1</v>
+      </c>
+      <c r="BX26" s="1">
+        <v>2</v>
+      </c>
+      <c r="BY26" s="1">
+        <v>3</v>
+      </c>
+      <c r="BZ26" s="1">
+        <v>4</v>
+      </c>
+      <c r="CA26" s="1">
+        <v>5</v>
+      </c>
+      <c r="CB26" s="1">
+        <v>6</v>
+      </c>
+      <c r="CC26" s="1">
+        <v>7</v>
+      </c>
+      <c r="CD26" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:89">
+      <c r="AU27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV27" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE27" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF27" s="1">
+        <v>2</v>
+      </c>
+      <c r="BG27" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH27" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI27" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ27" s="1">
+        <v>3</v>
+      </c>
+      <c r="BM27" s="1">
+        <v>8</v>
+      </c>
+      <c r="BN27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO27" s="1">
+        <v>8</v>
+      </c>
+      <c r="BP27" s="1">
+        <v>9</v>
+      </c>
+      <c r="BQ27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BW27" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX27" s="1">
+        <v>1</v>
+      </c>
+      <c r="BY27" s="1">
+        <v>2</v>
+      </c>
+      <c r="BZ27" s="1">
+        <v>3</v>
+      </c>
+      <c r="CA27" s="1">
+        <v>4</v>
+      </c>
+      <c r="CB27" s="1">
+        <v>5</v>
+      </c>
+      <c r="CC27" s="1">
+        <v>6</v>
+      </c>
+      <c r="CD27" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:89">
       <c r="C28" s="1">
         <v>1</v>
       </c>
@@ -13886,8 +14729,68 @@
       <c r="AI28" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:35">
+      <c r="AU28" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE28" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF28" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG28" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH28" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI28" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ28" s="1">
+        <v>2</v>
+      </c>
+      <c r="BM28" s="1">
+        <v>8</v>
+      </c>
+      <c r="BN28" s="1">
+        <v>9</v>
+      </c>
+      <c r="BO28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BP28" s="1">
+        <v>8</v>
+      </c>
+      <c r="BQ28" s="1">
+        <v>9</v>
+      </c>
+      <c r="BR28" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BX28" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY28" s="1">
+        <v>1</v>
+      </c>
+      <c r="BZ28" s="1">
+        <v>2</v>
+      </c>
+      <c r="CA28" s="1">
+        <v>3</v>
+      </c>
+      <c r="CB28" s="1">
+        <v>4</v>
+      </c>
+      <c r="CC28" s="1">
+        <v>5</v>
+      </c>
+      <c r="CD28" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:89">
       <c r="D29" s="1">
         <v>2</v>
       </c>
@@ -13972,8 +14875,56 @@
       <c r="AI29" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:35">
+      <c r="BF29" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG29" s="1">
+        <v>2</v>
+      </c>
+      <c r="BH29" s="1">
+        <v>4</v>
+      </c>
+      <c r="BI29" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ29" s="1">
+        <v>1</v>
+      </c>
+      <c r="BN29" s="1">
+        <v>8</v>
+      </c>
+      <c r="BO29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BQ29" s="1">
+        <v>8</v>
+      </c>
+      <c r="BR29" s="1">
+        <v>9</v>
+      </c>
+      <c r="BY29" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ29" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA29" s="1">
+        <v>2</v>
+      </c>
+      <c r="CB29" s="1">
+        <v>3</v>
+      </c>
+      <c r="CC29" s="1">
+        <v>4</v>
+      </c>
+      <c r="CD29" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:89">
       <c r="E30" s="1">
         <v>3</v>
       </c>
@@ -14046,8 +14997,59 @@
       <c r="AI30" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:35">
+      <c r="AU30" s="1">
+        <v>2</v>
+      </c>
+      <c r="AV30" s="1">
+        <v>2</v>
+      </c>
+      <c r="BF30" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG30" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH30" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI30" s="1">
+        <v>5</v>
+      </c>
+      <c r="BJ30" s="1">
+        <v>0</v>
+      </c>
+      <c r="BN30" s="1">
+        <v>9</v>
+      </c>
+      <c r="BO30" s="1">
+        <v>9</v>
+      </c>
+      <c r="BP30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BQ30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BR30" s="1">
+        <v>8</v>
+      </c>
+      <c r="BZ30" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA30" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB30" s="1">
+        <v>2</v>
+      </c>
+      <c r="CC30" s="1">
+        <v>3</v>
+      </c>
+      <c r="CD30" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:89">
       <c r="F31" s="1">
         <v>4</v>
       </c>
@@ -14108,8 +15110,56 @@
       <c r="AI31" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:35">
+      <c r="AU31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV31" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF31" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG31" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH31" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI31" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ31" s="1">
+        <v>6</v>
+      </c>
+      <c r="BN31" s="1">
+        <v>8</v>
+      </c>
+      <c r="BO31" s="1">
+        <v>8</v>
+      </c>
+      <c r="BP31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BQ31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="CA31" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB31" s="1">
+        <v>1</v>
+      </c>
+      <c r="CC31" s="1">
+        <v>2</v>
+      </c>
+      <c r="CD31" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:89">
       <c r="G32" s="1">
         <v>5</v>
       </c>
@@ -14158,8 +15208,54 @@
       <c r="AI32" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="3:35">
+      <c r="AU32" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV32" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF32" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG32" s="1">
+        <v>2</v>
+      </c>
+      <c r="BH32" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI32" s="1">
+        <v>3</v>
+      </c>
+      <c r="BJ32" s="1">
+        <v>5</v>
+      </c>
+      <c r="BN32" s="1">
+        <v>8</v>
+      </c>
+      <c r="BO32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BP32" s="1">
+        <v>9</v>
+      </c>
+      <c r="BQ32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BR32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="CB32" s="1">
+        <v>0</v>
+      </c>
+      <c r="CC32" s="1">
+        <v>1</v>
+      </c>
+      <c r="CD32" s="1">
+        <v>2</v>
+      </c>
+      <c r="CK32" s="2"/>
+    </row>
+    <row r="33" spans="3:112">
       <c r="H33" s="1">
         <v>6</v>
       </c>
@@ -14196,8 +15292,39 @@
       <c r="AI33" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="3:35">
+      <c r="BG33" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH33" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI33" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ33" s="1">
+        <v>4</v>
+      </c>
+      <c r="BO33" s="1">
+        <v>9</v>
+      </c>
+      <c r="BP33" s="1">
+        <v>8</v>
+      </c>
+      <c r="BQ33" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="CC33" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD33" s="1">
+        <v>1</v>
+      </c>
+      <c r="CK33" s="2"/>
+    </row>
+    <row r="34" spans="3:112">
       <c r="I34" s="1">
         <v>7</v>
       </c>
@@ -14222,8 +15349,39 @@
       <c r="AI34" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="3:35">
+      <c r="AU34" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG34" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH34" s="1">
+        <v>3</v>
+      </c>
+      <c r="BI34" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ34" s="1">
+        <v>3</v>
+      </c>
+      <c r="BO34" s="1">
+        <v>8</v>
+      </c>
+      <c r="BP34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BQ34" s="1">
+        <v>9</v>
+      </c>
+      <c r="BR34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CD34" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK34" s="2"/>
+    </row>
+    <row r="35" spans="3:112">
       <c r="J35" s="1">
         <v>8</v>
       </c>
@@ -14236,8 +15394,182 @@
       <c r="AI35" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="3:35">
+      <c r="AU35" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG35" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH35" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI35" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ35" s="1">
+        <v>2</v>
+      </c>
+      <c r="BO35" s="1">
+        <v>9</v>
+      </c>
+      <c r="BP35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BQ35" s="1">
+        <v>8</v>
+      </c>
+      <c r="BR35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="CK35" s="2"/>
+    </row>
+    <row r="36" spans="3:112">
+      <c r="BG36" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH36" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI36" s="1">
+        <v>4</v>
+      </c>
+      <c r="BJ36" s="1">
+        <v>1</v>
+      </c>
+      <c r="BO36" s="1">
+        <v>8</v>
+      </c>
+      <c r="BP36" s="1">
+        <v>9</v>
+      </c>
+      <c r="BQ36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR36" s="1">
+        <v>9</v>
+      </c>
+      <c r="BU36" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV36" s="1">
+        <v>1</v>
+      </c>
+      <c r="BW36" s="1">
+        <v>2</v>
+      </c>
+      <c r="BX36" s="1">
+        <v>3</v>
+      </c>
+      <c r="BY36" s="1">
+        <v>4</v>
+      </c>
+      <c r="BZ36" s="1">
+        <v>5</v>
+      </c>
+      <c r="CA36" s="1">
+        <v>6</v>
+      </c>
+      <c r="CB36" s="1">
+        <v>7</v>
+      </c>
+      <c r="CC36" s="1">
+        <v>0</v>
+      </c>
+      <c r="CD36" s="1">
+        <v>1</v>
+      </c>
+      <c r="CE36" s="1">
+        <v>2</v>
+      </c>
+      <c r="CF36" s="1">
+        <v>3</v>
+      </c>
+      <c r="CG36" s="1">
+        <v>4</v>
+      </c>
+      <c r="CH36" s="1">
+        <v>5</v>
+      </c>
+      <c r="CI36" s="1">
+        <v>6</v>
+      </c>
+      <c r="CJ36" s="1">
+        <v>7</v>
+      </c>
+      <c r="CK36" s="2">
+        <v>0</v>
+      </c>
+      <c r="CL36" s="1">
+        <v>1</v>
+      </c>
+      <c r="CM36" s="1">
+        <v>2</v>
+      </c>
+      <c r="CN36" s="1">
+        <v>3</v>
+      </c>
+      <c r="CO36" s="1">
+        <v>4</v>
+      </c>
+      <c r="CP36" s="1">
+        <v>5</v>
+      </c>
+      <c r="CQ36" s="1">
+        <v>6</v>
+      </c>
+      <c r="CR36" s="1">
+        <v>7</v>
+      </c>
+      <c r="CS36" s="1">
+        <v>0</v>
+      </c>
+      <c r="CT36" s="1">
+        <v>1</v>
+      </c>
+      <c r="CU36" s="1">
+        <v>2</v>
+      </c>
+      <c r="CV36" s="1">
+        <v>3</v>
+      </c>
+      <c r="CW36" s="1">
+        <v>4</v>
+      </c>
+      <c r="CX36" s="1">
+        <v>5</v>
+      </c>
+      <c r="CY36" s="1">
+        <v>6</v>
+      </c>
+      <c r="CZ36" s="1">
+        <v>7</v>
+      </c>
+      <c r="DA36" s="1">
+        <v>0</v>
+      </c>
+      <c r="DB36" s="1">
+        <v>1</v>
+      </c>
+      <c r="DC36" s="1">
+        <v>2</v>
+      </c>
+      <c r="DD36" s="1">
+        <v>3</v>
+      </c>
+      <c r="DE36" s="1">
+        <v>4</v>
+      </c>
+      <c r="DF36" s="1">
+        <v>5</v>
+      </c>
+      <c r="DG36" s="1">
+        <v>6</v>
+      </c>
+      <c r="DH36" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="3:112">
       <c r="C37" s="1">
         <v>2</v>
       </c>
@@ -14334,8 +15666,141 @@
       <c r="AI37" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="3:35">
+      <c r="AU37" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG37" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH37" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI37" s="1">
+        <v>3</v>
+      </c>
+      <c r="BJ37" s="1">
+        <v>0</v>
+      </c>
+      <c r="BO37" s="1">
+        <v>8</v>
+      </c>
+      <c r="BP37" s="1">
+        <v>8</v>
+      </c>
+      <c r="BQ37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BR37" s="1">
+        <v>8</v>
+      </c>
+      <c r="BV37" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW37" s="1">
+        <v>1</v>
+      </c>
+      <c r="BX37" s="1">
+        <v>2</v>
+      </c>
+      <c r="BY37" s="1">
+        <v>3</v>
+      </c>
+      <c r="BZ37" s="1">
+        <v>4</v>
+      </c>
+      <c r="CA37" s="1">
+        <v>5</v>
+      </c>
+      <c r="CB37" s="1">
+        <v>6</v>
+      </c>
+      <c r="CD37" s="1">
+        <v>0</v>
+      </c>
+      <c r="CE37" s="1">
+        <v>1</v>
+      </c>
+      <c r="CF37" s="1">
+        <v>2</v>
+      </c>
+      <c r="CG37" s="1">
+        <v>3</v>
+      </c>
+      <c r="CH37" s="1">
+        <v>4</v>
+      </c>
+      <c r="CI37" s="1">
+        <v>5</v>
+      </c>
+      <c r="CJ37" s="1">
+        <v>6</v>
+      </c>
+      <c r="CK37" s="2"/>
+      <c r="CL37" s="1">
+        <v>0</v>
+      </c>
+      <c r="CM37" s="1">
+        <v>1</v>
+      </c>
+      <c r="CN37" s="1">
+        <v>2</v>
+      </c>
+      <c r="CO37" s="1">
+        <v>3</v>
+      </c>
+      <c r="CP37" s="1">
+        <v>4</v>
+      </c>
+      <c r="CQ37" s="1">
+        <v>5</v>
+      </c>
+      <c r="CR37" s="1">
+        <v>6</v>
+      </c>
+      <c r="CT37" s="1">
+        <v>0</v>
+      </c>
+      <c r="CU37" s="1">
+        <v>1</v>
+      </c>
+      <c r="CV37" s="1">
+        <v>2</v>
+      </c>
+      <c r="CW37" s="1">
+        <v>3</v>
+      </c>
+      <c r="CX37" s="1">
+        <v>4</v>
+      </c>
+      <c r="CY37" s="1">
+        <v>5</v>
+      </c>
+      <c r="CZ37" s="1">
+        <v>6</v>
+      </c>
+      <c r="DB37" s="1">
+        <v>0</v>
+      </c>
+      <c r="DC37" s="1">
+        <v>1</v>
+      </c>
+      <c r="DD37" s="1">
+        <v>2</v>
+      </c>
+      <c r="DE37" s="1">
+        <v>3</v>
+      </c>
+      <c r="DF37" s="1">
+        <v>4</v>
+      </c>
+      <c r="DG37" s="1">
+        <v>5</v>
+      </c>
+      <c r="DH37" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="3:112">
       <c r="D38" s="1">
         <v>1</v>
       </c>
@@ -14420,8 +15885,117 @@
       <c r="AI38" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="3:35">
+      <c r="BH38" s="1">
+        <v>2</v>
+      </c>
+      <c r="BI38" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ38" s="1">
+        <v>5</v>
+      </c>
+      <c r="BP38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BQ38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BW38" s="1">
+        <v>0</v>
+      </c>
+      <c r="BX38" s="1">
+        <v>1</v>
+      </c>
+      <c r="BY38" s="1">
+        <v>2</v>
+      </c>
+      <c r="BZ38" s="1">
+        <v>3</v>
+      </c>
+      <c r="CA38" s="1">
+        <v>4</v>
+      </c>
+      <c r="CB38" s="1">
+        <v>5</v>
+      </c>
+      <c r="CE38" s="1">
+        <v>0</v>
+      </c>
+      <c r="CF38" s="1">
+        <v>1</v>
+      </c>
+      <c r="CG38" s="1">
+        <v>2</v>
+      </c>
+      <c r="CH38" s="1">
+        <v>3</v>
+      </c>
+      <c r="CI38" s="1">
+        <v>4</v>
+      </c>
+      <c r="CJ38" s="1">
+        <v>5</v>
+      </c>
+      <c r="CK38" s="2"/>
+      <c r="CM38" s="1">
+        <v>0</v>
+      </c>
+      <c r="CN38" s="1">
+        <v>1</v>
+      </c>
+      <c r="CO38" s="1">
+        <v>2</v>
+      </c>
+      <c r="CP38" s="1">
+        <v>3</v>
+      </c>
+      <c r="CQ38" s="1">
+        <v>4</v>
+      </c>
+      <c r="CR38" s="1">
+        <v>5</v>
+      </c>
+      <c r="CU38" s="1">
+        <v>0</v>
+      </c>
+      <c r="CV38" s="1">
+        <v>1</v>
+      </c>
+      <c r="CW38" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX38" s="1">
+        <v>3</v>
+      </c>
+      <c r="CY38" s="1">
+        <v>4</v>
+      </c>
+      <c r="CZ38" s="1">
+        <v>5</v>
+      </c>
+      <c r="DC38" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD38" s="1">
+        <v>1</v>
+      </c>
+      <c r="DE38" s="1">
+        <v>2</v>
+      </c>
+      <c r="DF38" s="1">
+        <v>3</v>
+      </c>
+      <c r="DG38" s="1">
+        <v>4</v>
+      </c>
+      <c r="DH38" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="3:112">
       <c r="E39" s="1">
         <v>0</v>
       </c>
@@ -14494,8 +16068,102 @@
       <c r="AI39" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="3:35">
+      <c r="BH39" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI39" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ39" s="1">
+        <v>4</v>
+      </c>
+      <c r="BP39" s="1">
+        <v>9</v>
+      </c>
+      <c r="BQ39" s="1">
+        <v>9</v>
+      </c>
+      <c r="BR39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BX39" s="1">
+        <v>0</v>
+      </c>
+      <c r="BY39" s="1">
+        <v>1</v>
+      </c>
+      <c r="BZ39" s="1">
+        <v>2</v>
+      </c>
+      <c r="CA39" s="1">
+        <v>3</v>
+      </c>
+      <c r="CB39" s="1">
+        <v>4</v>
+      </c>
+      <c r="CF39" s="1">
+        <v>0</v>
+      </c>
+      <c r="CG39" s="1">
+        <v>1</v>
+      </c>
+      <c r="CH39" s="1">
+        <v>2</v>
+      </c>
+      <c r="CI39" s="1">
+        <v>3</v>
+      </c>
+      <c r="CJ39" s="1">
+        <v>4</v>
+      </c>
+      <c r="CK39" s="2"/>
+      <c r="CN39" s="1">
+        <v>0</v>
+      </c>
+      <c r="CO39" s="1">
+        <v>1</v>
+      </c>
+      <c r="CP39" s="1">
+        <v>2</v>
+      </c>
+      <c r="CQ39" s="1">
+        <v>3</v>
+      </c>
+      <c r="CR39" s="1">
+        <v>4</v>
+      </c>
+      <c r="CV39" s="1">
+        <v>0</v>
+      </c>
+      <c r="CW39" s="1">
+        <v>1</v>
+      </c>
+      <c r="CX39" s="1">
+        <v>2</v>
+      </c>
+      <c r="CY39" s="1">
+        <v>3</v>
+      </c>
+      <c r="CZ39" s="1">
+        <v>4</v>
+      </c>
+      <c r="DD39" s="1">
+        <v>0</v>
+      </c>
+      <c r="DE39" s="1">
+        <v>1</v>
+      </c>
+      <c r="DF39" s="1">
+        <v>2</v>
+      </c>
+      <c r="DG39" s="1">
+        <v>3</v>
+      </c>
+      <c r="DH39" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="3:112">
       <c r="F40" s="1">
         <v>1</v>
       </c>
@@ -14556,8 +16224,87 @@
       <c r="AI40" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="3:35">
+      <c r="BH40" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI40" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ40" s="1">
+        <v>3</v>
+      </c>
+      <c r="BP40" s="1">
+        <v>8</v>
+      </c>
+      <c r="BQ40" s="1">
+        <v>8</v>
+      </c>
+      <c r="BR40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BY40" s="1">
+        <v>0</v>
+      </c>
+      <c r="BZ40" s="1">
+        <v>1</v>
+      </c>
+      <c r="CA40" s="1">
+        <v>2</v>
+      </c>
+      <c r="CB40" s="1">
+        <v>3</v>
+      </c>
+      <c r="CG40" s="1">
+        <v>0</v>
+      </c>
+      <c r="CH40" s="1">
+        <v>1</v>
+      </c>
+      <c r="CI40" s="1">
+        <v>2</v>
+      </c>
+      <c r="CJ40" s="1">
+        <v>3</v>
+      </c>
+      <c r="CK40" s="2"/>
+      <c r="CO40" s="1">
+        <v>0</v>
+      </c>
+      <c r="CP40" s="1">
+        <v>1</v>
+      </c>
+      <c r="CQ40" s="1">
+        <v>2</v>
+      </c>
+      <c r="CR40" s="1">
+        <v>3</v>
+      </c>
+      <c r="CW40" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX40" s="1">
+        <v>1</v>
+      </c>
+      <c r="CY40" s="1">
+        <v>2</v>
+      </c>
+      <c r="CZ40" s="1">
+        <v>3</v>
+      </c>
+      <c r="DE40" s="1">
+        <v>0</v>
+      </c>
+      <c r="DF40" s="1">
+        <v>1</v>
+      </c>
+      <c r="DG40" s="1">
+        <v>2</v>
+      </c>
+      <c r="DH40" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="3:112">
       <c r="G41" s="1">
         <v>2</v>
       </c>
@@ -14606,8 +16353,72 @@
       <c r="AI41" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="3:35">
+      <c r="BH41" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI41" s="1">
+        <v>3</v>
+      </c>
+      <c r="BJ41" s="1">
+        <v>2</v>
+      </c>
+      <c r="BP41" s="1">
+        <v>9</v>
+      </c>
+      <c r="BQ41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BR41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BZ41" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA41" s="1">
+        <v>1</v>
+      </c>
+      <c r="CB41" s="1">
+        <v>2</v>
+      </c>
+      <c r="CH41" s="1">
+        <v>0</v>
+      </c>
+      <c r="CI41" s="1">
+        <v>1</v>
+      </c>
+      <c r="CJ41" s="1">
+        <v>2</v>
+      </c>
+      <c r="CK41" s="2"/>
+      <c r="CP41" s="1">
+        <v>0</v>
+      </c>
+      <c r="CQ41" s="1">
+        <v>1</v>
+      </c>
+      <c r="CR41" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX41" s="1">
+        <v>0</v>
+      </c>
+      <c r="CY41" s="1">
+        <v>1</v>
+      </c>
+      <c r="CZ41" s="1">
+        <v>2</v>
+      </c>
+      <c r="DF41" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG41" s="1">
+        <v>1</v>
+      </c>
+      <c r="DH41" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:112">
       <c r="H42" s="1">
         <v>3</v>
       </c>
@@ -14644,8 +16455,57 @@
       <c r="AI42" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="3:35">
+      <c r="BH42" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI42" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ42" s="1">
+        <v>1</v>
+      </c>
+      <c r="BP42" s="1">
+        <v>8</v>
+      </c>
+      <c r="BQ42" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR42" s="1">
+        <v>9</v>
+      </c>
+      <c r="CA42" s="1">
+        <v>0</v>
+      </c>
+      <c r="CB42" s="1">
+        <v>1</v>
+      </c>
+      <c r="CI42" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ42" s="1">
+        <v>1</v>
+      </c>
+      <c r="CK42" s="2"/>
+      <c r="CQ42" s="1">
+        <v>0</v>
+      </c>
+      <c r="CR42" s="1">
+        <v>1</v>
+      </c>
+      <c r="CY42" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ42" s="1">
+        <v>1</v>
+      </c>
+      <c r="DG42" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="3:112">
       <c r="I43" s="1">
         <v>4</v>
       </c>
@@ -14670,8 +16530,42 @@
       <c r="AI43" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="3:35">
+      <c r="BH43" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI43" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ43" s="1">
+        <v>0</v>
+      </c>
+      <c r="BP43" s="1">
+        <v>8</v>
+      </c>
+      <c r="BQ43" s="1">
+        <v>9</v>
+      </c>
+      <c r="BR43" s="1">
+        <v>8</v>
+      </c>
+      <c r="CB43" s="1">
+        <v>0</v>
+      </c>
+      <c r="CJ43" s="1">
+        <v>0</v>
+      </c>
+      <c r="CK43" s="2"/>
+      <c r="CR43" s="1">
+        <v>0</v>
+      </c>
+      <c r="CZ43" s="1">
+        <v>0</v>
+      </c>
+      <c r="DH43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="3:112">
       <c r="J44" s="1">
         <v>5</v>
       </c>
@@ -14683,6 +16577,171 @@
       </c>
       <c r="AI44" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="BI44" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ44" s="1">
+        <v>4</v>
+      </c>
+      <c r="BQ44" s="1">
+        <v>8</v>
+      </c>
+      <c r="BR44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="CK44" s="2"/>
+    </row>
+    <row r="45" spans="3:112">
+      <c r="BI45" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ45" s="1">
+        <v>3</v>
+      </c>
+      <c r="BQ45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BR45" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CK45" s="2"/>
+    </row>
+    <row r="46" spans="3:112">
+      <c r="BI46" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ46" s="1">
+        <v>2</v>
+      </c>
+      <c r="BQ46" s="1">
+        <v>9</v>
+      </c>
+      <c r="BR46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="CK46" s="2"/>
+    </row>
+    <row r="47" spans="3:112">
+      <c r="BI47" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ47" s="1">
+        <v>1</v>
+      </c>
+      <c r="BQ47" s="1">
+        <v>8</v>
+      </c>
+      <c r="BR47" s="1">
+        <v>9</v>
+      </c>
+      <c r="CK47" s="2"/>
+    </row>
+    <row r="48" spans="3:112">
+      <c r="BI48" s="1">
+        <v>1</v>
+      </c>
+      <c r="BJ48" s="1">
+        <v>0</v>
+      </c>
+      <c r="BQ48" s="1">
+        <v>9</v>
+      </c>
+      <c r="BR48" s="1">
+        <v>8</v>
+      </c>
+      <c r="CK48" s="2"/>
+    </row>
+    <row r="49" spans="61:70">
+      <c r="BI49" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ49" s="1">
+        <v>3</v>
+      </c>
+      <c r="BQ49" s="1">
+        <v>8</v>
+      </c>
+      <c r="BR49" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="61:70">
+      <c r="BI50" s="1">
+        <v>0</v>
+      </c>
+      <c r="BJ50" s="1">
+        <v>2</v>
+      </c>
+      <c r="BQ50" s="1">
+        <v>8</v>
+      </c>
+      <c r="BR50" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="61:70">
+      <c r="BJ51" s="1">
+        <v>1</v>
+      </c>
+      <c r="BR51" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="61:70">
+      <c r="BJ52" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR52" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="61:70">
+      <c r="BJ53" s="1">
+        <v>2</v>
+      </c>
+      <c r="BR53" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="61:70">
+      <c r="BJ54" s="1">
+        <v>1</v>
+      </c>
+      <c r="BR54" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="61:70">
+      <c r="BJ55" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR55" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="61:70">
+      <c r="BJ56" s="1">
+        <v>1</v>
+      </c>
+      <c r="BR56" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="61:70">
+      <c r="BJ57" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR57" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="61:70">
+      <c r="BJ58" s="1">
+        <v>0</v>
+      </c>
+      <c r="BR58" s="1">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -14694,12 +16753,1070 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="D1:BG12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AJ5" sqref="AJ5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="7" max="7" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="4:59">
+      <c r="W1">
+        <v>1</v>
+      </c>
+      <c r="Y1">
+        <v>2</v>
+      </c>
+      <c r="AA1">
+        <v>3</v>
+      </c>
+      <c r="AC1">
+        <v>4</v>
+      </c>
+      <c r="AE1">
+        <v>5</v>
+      </c>
+      <c r="AG1">
+        <v>6</v>
+      </c>
+      <c r="AI1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="4:59">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>6</v>
+      </c>
+      <c r="S3">
+        <v>7</v>
+      </c>
+      <c r="U3">
+        <v>8</v>
+      </c>
+      <c r="W3">
+        <v>9</v>
+      </c>
+      <c r="Y3">
+        <v>10</v>
+      </c>
+      <c r="AA3">
+        <v>11</v>
+      </c>
+      <c r="AC3">
+        <v>12</v>
+      </c>
+      <c r="AE3">
+        <v>13</v>
+      </c>
+      <c r="AG3">
+        <v>14</v>
+      </c>
+      <c r="AI3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="4:59">
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>6</v>
+      </c>
+      <c r="K5" s="1">
+        <v>7</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="N5" s="1">
+        <v>2</v>
+      </c>
+      <c r="O5" s="1">
+        <v>3</v>
+      </c>
+      <c r="P5" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>5</v>
+      </c>
+      <c r="R5" s="1">
+        <v>6</v>
+      </c>
+      <c r="S5" s="1">
+        <v>7</v>
+      </c>
+      <c r="T5" s="1">
+        <v>0</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1</v>
+      </c>
+      <c r="V5" s="1">
+        <v>2</v>
+      </c>
+      <c r="W5" s="1">
+        <v>3</v>
+      </c>
+      <c r="X5" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>7</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>7</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AM5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AN5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AO5" s="1">
+        <v>5</v>
+      </c>
+      <c r="AP5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AQ5" s="1">
+        <v>7</v>
+      </c>
+      <c r="AR5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AT5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AU5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AV5" s="1">
+        <v>4</v>
+      </c>
+      <c r="AW5" s="1">
+        <v>5</v>
+      </c>
+      <c r="AX5" s="1">
+        <v>6</v>
+      </c>
+      <c r="AY5" s="1">
+        <v>7</v>
+      </c>
+      <c r="AZ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="1">
+        <v>1</v>
+      </c>
+      <c r="BB5" s="1">
+        <v>2</v>
+      </c>
+      <c r="BC5" s="1">
+        <v>3</v>
+      </c>
+      <c r="BD5" s="1">
+        <v>4</v>
+      </c>
+      <c r="BE5" s="1">
+        <v>5</v>
+      </c>
+      <c r="BF5" s="1">
+        <v>6</v>
+      </c>
+      <c r="BG5" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="4:59">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1">
+        <v>6</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>2</v>
+      </c>
+      <c r="P6" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>4</v>
+      </c>
+      <c r="R6" s="1">
+        <v>5</v>
+      </c>
+      <c r="S6" s="1">
+        <v>6</v>
+      </c>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1">
+        <v>1</v>
+      </c>
+      <c r="W6" s="1">
+        <v>2</v>
+      </c>
+      <c r="X6" s="1">
+        <v>3</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>5</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>5</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AN6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>5</v>
+      </c>
+      <c r="AQ6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AU6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AV6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AW6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AX6" s="1">
+        <v>5</v>
+      </c>
+      <c r="AY6" s="1">
+        <v>6</v>
+      </c>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="1">
+        <v>1</v>
+      </c>
+      <c r="BC6" s="1">
+        <v>2</v>
+      </c>
+      <c r="BD6" s="1">
+        <v>3</v>
+      </c>
+      <c r="BE6" s="1">
+        <v>4</v>
+      </c>
+      <c r="BF6" s="1">
+        <v>5</v>
+      </c>
+      <c r="BG6" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="4:59">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1">
+        <v>4</v>
+      </c>
+      <c r="K7" s="1">
+        <v>5</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>3</v>
+      </c>
+      <c r="R7" s="1">
+        <v>4</v>
+      </c>
+      <c r="S7" s="1">
+        <v>5</v>
+      </c>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1">
+        <v>0</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1</v>
+      </c>
+      <c r="X7" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AN7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AO7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AP7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AQ7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AR7" s="1"/>
+      <c r="AS7" s="1"/>
+      <c r="AT7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV7" s="1">
+        <v>2</v>
+      </c>
+      <c r="AW7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AX7" s="1">
+        <v>4</v>
+      </c>
+      <c r="AY7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
+      <c r="BB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD7" s="1">
+        <v>2</v>
+      </c>
+      <c r="BE7" s="1">
+        <v>3</v>
+      </c>
+      <c r="BF7" s="1">
+        <v>4</v>
+      </c>
+      <c r="BG7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="4:59">
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1">
+        <v>3</v>
+      </c>
+      <c r="K8" s="1">
+        <v>4</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1">
+        <v>0</v>
+      </c>
+      <c r="P8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>2</v>
+      </c>
+      <c r="R8" s="1">
+        <v>3</v>
+      </c>
+      <c r="S8" s="1">
+        <v>4</v>
+      </c>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AO8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AP8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AQ8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AX8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AY8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="1">
+        <v>1</v>
+      </c>
+      <c r="BE8" s="1">
+        <v>2</v>
+      </c>
+      <c r="BF8" s="1">
+        <v>3</v>
+      </c>
+      <c r="BG8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="4:59">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1">
+        <v>2</v>
+      </c>
+      <c r="S9" s="1">
+        <v>3</v>
+      </c>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AI9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AP9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AQ9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AR9" s="1"/>
+      <c r="AS9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AX9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AY9" s="1">
+        <v>3</v>
+      </c>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="1"/>
+      <c r="BC9" s="1"/>
+      <c r="BD9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF9" s="1">
+        <v>2</v>
+      </c>
+      <c r="BG9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:59">
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="R10" s="1">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1">
+        <v>2</v>
+      </c>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="1"/>
+      <c r="AO10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AQ10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="1"/>
+      <c r="BC10" s="1"/>
+      <c r="BD10" s="1"/>
+      <c r="BE10" s="1">
+        <v>0</v>
+      </c>
+      <c r="BF10" s="1">
+        <v>1</v>
+      </c>
+      <c r="BG10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:59">
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>1</v>
+      </c>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="1"/>
+      <c r="BC11" s="1"/>
+      <c r="BD11" s="1"/>
+      <c r="BE11" s="1"/>
+      <c r="BF11" s="1">
+        <v>0</v>
+      </c>
+      <c r="BG11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="4:59">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="1"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="1"/>
+      <c r="AY12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="1"/>
+      <c r="BC12" s="1"/>
+      <c r="BD12" s="1"/>
+      <c r="BE12" s="1"/>
+      <c r="BF12" s="1"/>
+      <c r="BG12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>